<commit_message>
We start implementing tbl_summary and make aesthetic changes to all our boxplot/points. We add plots for ablation time, irrigation delivered, energy on time, and VCAS-II plots
</commit_message>
<xml_diff>
--- a/data/raw/12_26_24_VCAS-rove_time.xlsx
+++ b/data/raw/12_26_24_VCAS-rove_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AA86111-7897-6743-AA81-0C5B752FC7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8E161A5-A3AF-EB41-BD19-A6D56810D913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="164">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>This doesn't work correctly if done across days</t>
-  </si>
-  <si>
-    <t>procedure_time</t>
   </si>
   <si>
     <t>Ablation after VT induction</t>
@@ -864,7 +861,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="90">
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -1133,9 +1130,6 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
@@ -1158,11 +1152,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:H39" totalsRowShown="0">
-  <autoFilter ref="A1:H39" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="subjectId" dataDxfId="90"/>
-    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:G39" totalsRowShown="0">
+  <autoFilter ref="A1:G39" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="subjectId" dataDxfId="89"/>
     <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="88"/>
     <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="87">
       <calculatedColumnFormula>'1-001'!H35</calculatedColumnFormula>
@@ -2007,7 +2000,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -2017,12 +2010,12 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2032,47 +2025,47 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2582,14 +2575,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245153456[time_diff]))*3600 + MINUTE(SUM(Table245153456[time_diff])) * 60 + SECOND(SUM(Table245153456[time_diff]))</f>
         <v>332</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -2673,7 +2666,7 @@
         <v>1.6203703703704386E-4</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -2695,7 +2688,7 @@
         <v>1.2731481481481621E-4</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -2717,7 +2710,7 @@
         <v>1.9675925925932702E-4</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -3145,14 +3138,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515345[time_diff]))*3600 + MINUTE(SUM(Table24515345[time_diff])) * 60 + SECOND(SUM(Table24515345[time_diff]))</f>
         <v>63</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -3293,7 +3286,7 @@
         <v>2.1990740740740478E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -3702,14 +3695,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451534[time_diff]))*3600 + MINUTE(SUM(Table2451534[time_diff])) * 60 + SECOND(SUM(Table2451534[time_diff]))</f>
         <v>270</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -3808,7 +3801,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -4247,14 +4240,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245153[time_diff]))*3600 + MINUTE(SUM(Table245153[time_diff])) * 60 + SECOND(SUM(Table245153[time_diff]))</f>
         <v>211</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -4338,7 +4331,7 @@
         <v>2.418981481481508E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="14">
         <v>0.71141203703703704</v>
@@ -4364,7 +4357,7 @@
         <v>6.3888888888888884E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="16">
         <v>0.52440972222222226</v>
@@ -4388,7 +4381,7 @@
         <v>1.215277777777779E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -4793,14 +4786,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
         <v>1993</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6" t="e">
@@ -4962,7 +4955,7 @@
         <v>1.4004629629629645E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -5366,14 +5359,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2410[time_diff]))*3600 + MINUTE(SUM(Table2410[time_diff])) * 60 + SECOND(SUM(Table2410[time_diff]))</f>
         <v>1734</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -5939,14 +5932,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table249[time_diff]))*3600 + MINUTE(SUM(Table249[time_diff])) * 60 + SECOND(SUM(Table249[time_diff]))</f>
         <v>463</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -6068,7 +6061,7 @@
         <v>8.2870370370370372E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="14">
         <v>7.2511574074074076E-2</v>
@@ -6081,7 +6074,7 @@
         <v>1.4675925925925926E-2</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -6096,7 +6089,7 @@
         <v>6.7824074074074314E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="16">
         <v>8.9803240740740739E-2</v>
@@ -6122,7 +6115,7 @@
         <v>7.0370370370369528E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -6524,14 +6517,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24511[time_diff]))*3600 + MINUTE(SUM(Table24511[time_diff])) * 60 + SECOND(SUM(Table24511[time_diff]))</f>
         <v>2043</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -7084,14 +7077,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245[time_diff]))*3600 + MINUTE(SUM(Table245[time_diff])) * 60 + SECOND(SUM(Table245[time_diff]))</f>
         <v>568</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -7215,7 +7208,7 @@
         <v>1.4918981481481408E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="14">
         <v>0.80343750000000003</v>
@@ -7241,7 +7234,7 @@
         <v>2.1875000000000089E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" s="16">
         <v>0.81846064814814812</v>
@@ -7254,7 +7247,7 @@
         <v>1.4780092592592609E-2</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -7690,14 +7683,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245154[time_diff]))*3600 + MINUTE(SUM(Table245154[time_diff])) * 60 + SECOND(SUM(Table245154[time_diff]))</f>
         <v>1478</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -7754,687 +7747,656 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" style="6" hidden="1" customWidth="1"/>
-    <col min="3" max="5" width="11.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="53.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="2" max="4" width="11.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6">
-        <v>21600</v>
+        <v>2801</v>
       </c>
       <c r="C2" s="6">
-        <v>2801</v>
-      </c>
-      <c r="D2" s="6">
         <v>6452</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E2" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="6">
-        <v>17100</v>
+        <v>3965</v>
       </c>
       <c r="C3" s="6">
-        <v>3965</v>
-      </c>
-      <c r="D3" s="6">
         <v>5536</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="6">
+        <v>126</v>
+      </c>
+      <c r="B4" s="6">
         <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="6">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="6">
-        <v>57</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="6">
+        <v>2075</v>
+      </c>
       <c r="C6" s="6">
-        <v>2075</v>
-      </c>
-      <c r="D6" s="6">
         <v>5374</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E6" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="6">
+        <v>332</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="6">
         <v>63</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="6">
-        <v>332</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="6">
-        <v>63</v>
+      <c r="D8" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="6">
+        <v>270</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="6">
-        <v>270</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="D10" s="6" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>17760</v>
-      </c>
-      <c r="C11" s="6">
         <v>1993</v>
       </c>
-      <c r="D11" s="21">
+      <c r="C11" s="21">
         <v>8040</v>
       </c>
+      <c r="D11" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="D12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="6">
-        <v>8880</v>
+        <v>1734</v>
       </c>
       <c r="C13" s="6">
-        <v>1734</v>
-      </c>
-      <c r="D13" s="6">
         <v>2919</v>
       </c>
+      <c r="D13" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E13" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="6">
-        <v>8760</v>
+        <v>463</v>
       </c>
       <c r="C14" s="6">
-        <v>463</v>
-      </c>
-      <c r="D14" s="6">
         <v>2160</v>
       </c>
+      <c r="D14" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="E14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2043</v>
+      </c>
+      <c r="C15" s="6">
+        <v>4175</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="6">
+        <v>568</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1284</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1478</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2938</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2486</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3752</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2808</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3937</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3340</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2171</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="B23" s="6">
+        <v>2594</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2173</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="6">
-        <v>12840</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2043</v>
-      </c>
-      <c r="D15" s="6">
-        <v>4175</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="6">
+        <v>935</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2940</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="6">
+        <v>3180</v>
+      </c>
+      <c r="C25" s="6">
+        <v>7079</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="6">
-        <v>9600</v>
-      </c>
-      <c r="C16" s="6">
-        <v>568</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1284</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="E25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="6">
-        <v>10020</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1478</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2938</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="E26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="6">
+        <v>304</v>
+      </c>
+      <c r="C27" s="6">
+        <v>946</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="6">
-        <v>11340</v>
-      </c>
-      <c r="C18" s="6">
-        <v>2486</v>
-      </c>
-      <c r="D18" s="6">
-        <v>3752</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2808</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="6">
-        <v>3937</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="6">
-        <v>3340</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="6">
-        <v>2171</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="6">
-        <v>2594</v>
-      </c>
-      <c r="D23" s="6">
-        <v>2173</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="6">
-        <v>935</v>
-      </c>
-      <c r="D24" s="6">
-        <v>2940</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C25" s="6">
-        <v>3180</v>
-      </c>
-      <c r="D25" s="6">
-        <v>7079</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="E27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>144</v>
       </c>
-      <c r="C27" s="6">
-        <v>304</v>
-      </c>
-      <c r="D27" s="6">
-        <v>946</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>145</v>
+      <c r="B28" s="6">
+        <v>1338</v>
       </c>
       <c r="C28" s="6">
-        <v>1338</v>
-      </c>
-      <c r="D28" s="6">
         <v>2104</v>
       </c>
+      <c r="D28" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E28" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="4"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
-    <hyperlink ref="H13" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
-    <hyperlink ref="H15" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
-    <hyperlink ref="H16" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
-    <hyperlink ref="H20" r:id="rId9" xr:uid="{A6808D0E-445B-4C43-B4CD-98A767AEB45B}"/>
-    <hyperlink ref="H21" r:id="rId10" xr:uid="{1DF6C634-3492-DF49-9B55-296CB7CE64EB}"/>
-    <hyperlink ref="H22" r:id="rId11" xr:uid="{A85B1F2E-045A-B349-B848-E27125F76862}"/>
-    <hyperlink ref="H23" r:id="rId12" xr:uid="{F06AF91C-D4F5-BD4C-9E18-976763431CA8}"/>
-    <hyperlink ref="H24" r:id="rId13" xr:uid="{95E2EE1A-30AE-7C4A-82F1-ED430130C367}"/>
-    <hyperlink ref="H19" r:id="rId14" xr:uid="{AF18FFE3-5AD8-8B48-8774-27DF0448ED9B}"/>
-    <hyperlink ref="H17" r:id="rId15" xr:uid="{35914E4E-7CCE-DE4A-A86A-0832DC959DC1}"/>
-    <hyperlink ref="H18" r:id="rId16" xr:uid="{784B45B9-C4BE-7D45-8FB1-6D503B59F376}"/>
-    <hyperlink ref="H4" r:id="rId17" xr:uid="{C0B8A36A-046E-3141-9017-4AC27F374259}"/>
-    <hyperlink ref="H5" r:id="rId18" xr:uid="{ADB51FDF-90FB-8A45-AA7E-18F05E1E9EB4}"/>
-    <hyperlink ref="H7" r:id="rId19" xr:uid="{11FD46F8-273A-E846-8AC0-C83F764C748C}"/>
-    <hyperlink ref="H8" r:id="rId20" xr:uid="{4FCC054F-5CCF-1E42-9C0C-99382735F0ED}"/>
-    <hyperlink ref="H9" r:id="rId21" xr:uid="{37826A8D-6640-404E-875A-27B18FF4D5C9}"/>
-    <hyperlink ref="H10" r:id="rId22" xr:uid="{DF13A713-B84F-2745-A551-24144146FC0C}"/>
-    <hyperlink ref="H25" r:id="rId23" xr:uid="{0AED20DD-F5D7-9E4F-B740-8DE91A23F30A}"/>
-    <hyperlink ref="H26" r:id="rId24" xr:uid="{4BB18C29-3E47-F944-B221-2FBC408E879F}"/>
-    <hyperlink ref="H27" r:id="rId25" xr:uid="{D1899722-4A7F-C740-9D85-BB0987A5689C}"/>
-    <hyperlink ref="H28" r:id="rId26" xr:uid="{238BB9F0-EE8E-7B41-B4BB-814C938F8075}"/>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
+    <hyperlink ref="G11" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
+    <hyperlink ref="G15" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
+    <hyperlink ref="G16" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
+    <hyperlink ref="G20" r:id="rId9" xr:uid="{A6808D0E-445B-4C43-B4CD-98A767AEB45B}"/>
+    <hyperlink ref="G21" r:id="rId10" xr:uid="{1DF6C634-3492-DF49-9B55-296CB7CE64EB}"/>
+    <hyperlink ref="G22" r:id="rId11" xr:uid="{A85B1F2E-045A-B349-B848-E27125F76862}"/>
+    <hyperlink ref="G23" r:id="rId12" xr:uid="{F06AF91C-D4F5-BD4C-9E18-976763431CA8}"/>
+    <hyperlink ref="G24" r:id="rId13" xr:uid="{95E2EE1A-30AE-7C4A-82F1-ED430130C367}"/>
+    <hyperlink ref="G19" r:id="rId14" xr:uid="{AF18FFE3-5AD8-8B48-8774-27DF0448ED9B}"/>
+    <hyperlink ref="G17" r:id="rId15" xr:uid="{35914E4E-7CCE-DE4A-A86A-0832DC959DC1}"/>
+    <hyperlink ref="G18" r:id="rId16" xr:uid="{784B45B9-C4BE-7D45-8FB1-6D503B59F376}"/>
+    <hyperlink ref="G4" r:id="rId17" xr:uid="{C0B8A36A-046E-3141-9017-4AC27F374259}"/>
+    <hyperlink ref="G5" r:id="rId18" xr:uid="{ADB51FDF-90FB-8A45-AA7E-18F05E1E9EB4}"/>
+    <hyperlink ref="G7" r:id="rId19" xr:uid="{11FD46F8-273A-E846-8AC0-C83F764C748C}"/>
+    <hyperlink ref="G8" r:id="rId20" xr:uid="{4FCC054F-5CCF-1E42-9C0C-99382735F0ED}"/>
+    <hyperlink ref="G9" r:id="rId21" xr:uid="{37826A8D-6640-404E-875A-27B18FF4D5C9}"/>
+    <hyperlink ref="G10" r:id="rId22" xr:uid="{DF13A713-B84F-2745-A551-24144146FC0C}"/>
+    <hyperlink ref="G25" r:id="rId23" xr:uid="{0AED20DD-F5D7-9E4F-B740-8DE91A23F30A}"/>
+    <hyperlink ref="G26" r:id="rId24" xr:uid="{4BB18C29-3E47-F944-B221-2FBC408E879F}"/>
+    <hyperlink ref="G27" r:id="rId25" xr:uid="{D1899722-4A7F-C740-9D85-BB0987A5689C}"/>
+    <hyperlink ref="G28" r:id="rId26" xr:uid="{238BB9F0-EE8E-7B41-B4BB-814C938F8075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8494,7 +8456,7 @@
         <v>1.8287037037036935E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="14">
         <v>0.64094907407407409</v>
@@ -8520,7 +8482,7 @@
         <v>6.5393518518518379E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="16">
         <v>0.6681597222222222</v>
@@ -8971,14 +8933,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515416[time_diff]))*3600 + MINUTE(SUM(Table24515416[time_diff])) * 60 + SECOND(SUM(Table24515416[time_diff]))</f>
         <v>2486</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -9090,7 +9052,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -9537,14 +9499,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451517181920[time_diff]))*3600 + MINUTE(SUM(Table2451517181920[time_diff])) * 60 + SECOND(SUM(Table2451517181920[time_diff]))</f>
         <v>2808</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -9628,7 +9590,7 @@
         <v>3.4502314814814805E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -9637,7 +9599,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -10088,14 +10050,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515171819[time_diff]))*3600 + MINUTE(SUM(Table24515171819[time_diff])) * 60 + SECOND(SUM(Table24515171819[time_diff]))</f>
         <v>3937</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -10179,7 +10141,7 @@
         <v>3.0567129629629652E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -10188,7 +10150,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -10639,14 +10601,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245151718[time_diff]))*3600 + MINUTE(SUM(Table245151718[time_diff])) * 60 + SECOND(SUM(Table245151718[time_diff]))</f>
         <v>3340</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -10736,7 +10698,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -11187,14 +11149,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451517[time_diff]))*3600 + MINUTE(SUM(Table2451517[time_diff])) * 60 + SECOND(SUM(Table2451517[time_diff]))</f>
         <v>2171</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -11733,14 +11695,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451521[time_diff]))*3600 + MINUTE(SUM(Table2451521[time_diff])) * 60 + SECOND(SUM(Table2451521[time_diff]))</f>
         <v>2594</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -12279,14 +12241,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245152122[time_diff]))*3600 + MINUTE(SUM(Table245152122[time_diff])) * 60 + SECOND(SUM(Table245152122[time_diff]))</f>
         <v>935</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -12370,7 +12332,7 @@
         <v>1.9791666666666652E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="14">
         <v>0.50756944444444441</v>
@@ -12383,7 +12345,7 @@
         <v>7.3564814814814805E-2</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -12398,7 +12360,7 @@
         <v>2.4305555555559355E-4</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" s="16">
         <v>0.58136574074074077</v>
@@ -12424,7 +12386,7 @@
         <v>1.3194444444444287E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="14">
         <v>0.58384259259259264</v>
@@ -12450,7 +12412,7 @@
         <v>7.0601851851859188E-4</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -12472,7 +12434,7 @@
         <v>2.9976851851851727E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -12494,7 +12456,7 @@
         <v>1.5277777777777946E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -12516,7 +12478,7 @@
         <v>1.6087962962962887E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -12538,7 +12500,7 @@
         <v>2.0601851851852482E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -12560,7 +12522,7 @@
         <v>2.4421296296296413E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -12582,7 +12544,7 @@
         <v>2.2106481481481977E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -12604,7 +12566,7 @@
         <v>2.1990740740740478E-4</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -12626,7 +12588,7 @@
         <v>1.5046296296294948E-4</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -12648,7 +12610,7 @@
         <v>1.5277777777777946E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -12922,14 +12884,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451529[time_diff]))*3600 + MINUTE(SUM(Table2451529[time_diff])) * 60 + SECOND(SUM(Table2451529[time_diff]))</f>
         <v>3180</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -13460,14 +13422,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245152930[time_diff]))*3600 + MINUTE(SUM(Table245152930[time_diff])) * 60 + SECOND(SUM(Table245152930[time_diff]))</f>
         <v>0</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -13551,7 +13513,7 @@
         <v>4.5138888888895945E-4</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2" s="14">
         <v>0.85078703703703706</v>
@@ -13577,7 +13539,7 @@
         <v>3.067129629629628E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -14016,14 +13978,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245152931[time_diff]))*3600 + MINUTE(SUM(Table245152931[time_diff])) * 60 + SECOND(SUM(Table245152931[time_diff]))</f>
         <v>304</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -14554,14 +14516,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515[time_diff]))*3600 + MINUTE(SUM(Table24515[time_diff])) * 60 + SECOND(SUM(Table24515[time_diff]))</f>
         <v>0</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -14645,7 +14607,7 @@
         <v>1.4490740740740748E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F2" s="14">
         <v>0.64076388888888891</v>
@@ -15115,14 +15077,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515293132[time_diff]))*3600 + MINUTE(SUM(Table24515293132[time_diff])) * 60 + SECOND(SUM(Table24515293132[time_diff]))</f>
         <v>1338</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -15576,14 +15538,14 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2[time_diff]))*3600 + MINUTE(SUM(Table2[time_diff])) * 60 + SECOND(SUM(Table2[time_diff]))</f>
         <v>2801</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" s="6">
         <f>HOUR(SUM(Table213[time_diff]))*3600 + MINUTE(SUM(Table213[time_diff])) * 60 + SECOND(SUM(Table213[time_diff]))</f>
@@ -15687,7 +15649,7 @@
         <v>1.4351851851851921E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="4">
         <v>9.087962962962963E-2</v>
@@ -15712,7 +15674,7 @@
         <v>4.1666666666666657E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="4">
         <f>Table21314[[#This Row],[end_time]]-Table21314[[#This Row],[start_time]]</f>
@@ -15731,7 +15693,7 @@
         <v>5.277777777777784E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -16107,14 +16069,14 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table246[time_diff]))*3600 + MINUTE(SUM(Table246[time_diff])) * 60 + SECOND(SUM(Table246[time_diff]))</f>
         <v>3965</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" s="6">
         <f>HOUR(SUM(Table21314[time_diff]))*3600 + MINUTE(SUM(Table21314[time_diff])) * 60 + SECOND(SUM(Table21314[time_diff]))</f>
@@ -16678,14 +16640,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515345678[time_diff]))*3600 + MINUTE(SUM(Table24515345678[time_diff])) * 60 + SECOND(SUM(Table24515345678[time_diff]))</f>
         <v>11</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -16769,7 +16731,7 @@
         <v>1.9675925925927151E-4</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -17227,14 +17189,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451534567[time_diff]))*3600 + MINUTE(SUM(Table2451534567[time_diff])) * 60 + SECOND(SUM(Table2451534567[time_diff]))</f>
         <v>57</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -17344,7 +17306,7 @@
         <v>1.3425925925926174E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="16">
         <v>0.63871527777777781</v>
@@ -17370,7 +17332,7 @@
         <v>6.1111111111110672E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="14">
         <v>0.66612268518518514</v>
@@ -17396,7 +17358,7 @@
         <v>2.8819444444444448E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="16">
         <v>0.69787037037037036</v>
@@ -17782,14 +17744,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table247[time_diff]))*3600 + MINUTE(SUM(Table247[time_diff])) * 60 + SECOND(SUM(Table247[time_diff]))</f>
         <v>2075</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -17999,7 +17961,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -18140,7 +18102,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24812[time_diff]))*3600 + MINUTE(SUM(Table24812[time_diff])) * 60 + SECOND(SUM(Table24812[time_diff]))</f>

</xml_diff>